<commit_message>
Updated Class_2_Weights and References
V_n_diagram.m
-fixed some unit conversions
-updated print statements
Class_2_Weights.m
-added variables from other scripts
-updated weight estimates
</commit_message>
<xml_diff>
--- a/Aircraft_Weight.xlsx
+++ b/Aircraft_Weight.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -393,7 +393,7 @@
         <v>920</v>
       </c>
       <c r="B3">
-        <v>28726708.264966652</v>
+        <v>5205.1047343495065</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -401,7 +401,7 @@
         <v>34652.716349358925</v>
       </c>
       <c r="B4">
-        <v>949</v>
+        <v>1081.8259261871792</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -409,7 +409,7 @@
         <v>3709.7488512462119</v>
       </c>
       <c r="B5">
-        <v>920</v>
+        <v>293.2384891592568</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -417,7 +417,7 @@
         <v>356.22123211615428</v>
       </c>
       <c r="B6">
-        <v>34652.716349358925</v>
+        <v>5971.3297340435647</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -449,7 +449,7 @@
         <v>869.72022940324428</v>
       </c>
       <c r="B10">
-        <v>28769715.188977543</v>
+        <v>19036.706545269397</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -571,7 +571,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26">
-        <v>28789923.678632636</v>
+        <v>39245.196200359991</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Class 2 Weight Update
Supersonic_Aircraft_Design.m
-Updated operating empty weight calculations
Class_2_Weights
-Came up with estimate for new WTO and compared to preliminary sizing
value.
</commit_message>
<xml_diff>
--- a/Aircraft_Weight.xlsx
+++ b/Aircraft_Weight.xlsx
@@ -497,7 +497,7 @@
         <v>1716.009097668513</v>
       </c>
       <c r="B16">
-        <v>718.91891891891896</v>
+        <v>1335.1351351351352</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -553,7 +553,7 @@
         <v>308.10810810810813</v>
       </c>
       <c r="B23">
-        <v>1.3339253901309587</v>
+        <v>6.5250839517241932</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -561,17 +561,17 @@
         <v>28789923.678632636</v>
       </c>
       <c r="B24">
-        <v>136</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25">
-        <v>308.10810810810813</v>
+        <v>513.51351351351354</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26">
-        <v>39245.196200359991</v>
+        <v>41839.193104738762</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>